<commit_message>
Fix indentation errors in vehicles.py km processing loops
</commit_message>
<xml_diff>
--- a/Vaka formu v2.xlsx
+++ b/Vaka formu v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osman\Desktop\HEALMEDY\ABROV2\lockdownsofthbys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE83AB7-E041-4962-93F3-4A67842C7A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C400938A-4AA0-48F5-BC3B-ED08C82E682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F7866268-8B2F-44D8-8CBE-F8EBB83B2119}"/>
   </bookViews>
@@ -2921,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A227F368-0EB9-4EDF-A758-79521A3623E2}">
   <dimension ref="A1:AA80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:J7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>